<commit_message>
Intent, Moved models to public directory
</commit_message>
<xml_diff>
--- a/public/intent-definition.xlsx
+++ b/public/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40107479-4AD8-4796-BCAE-80904BDB6F3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A842882-97B6-4994-9922-C67D6CA70791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="452" uniqueCount="227">
   <si>
     <t>intent_name</t>
   </si>
@@ -688,9 +688,6 @@
     <t>tl</t>
   </si>
   <si>
-    <t>Hello,Hi,Wow,Power</t>
-  </si>
-  <si>
     <t>I want to die</t>
   </si>
   <si>
@@ -704,6 +701,12 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>sys.age:1,sys.name:0</t>
+  </si>
+  <si>
+    <t>My name is {@name:Steven}</t>
   </si>
 </sst>
 </file>
@@ -3835,7 +3838,7 @@
   <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3855,10 +3858,10 @@
         <v>215</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>213</v>
@@ -3902,10 +3905,13 @@
         <v>216</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>222</v>
+        <v>221</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -3928,12 +3934,12 @@
         <v>216</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="J7" s="1" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Custom Prompts for Entities, Added value, isList properties for setting parameters
</commit_message>
<xml_diff>
--- a/public/intent-definition.xlsx
+++ b/public/intent-definition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\User\Documents\Code\Thesis\Symptom-Checker-Chatbot\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705E4F47-C95D-4359-804A-ACE81EF32F46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C56260B-B64D-4BF7-96A3-B6F1E48B0A47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="450" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="252">
   <si>
     <t>intent_name</t>
   </si>
@@ -713,13 +713,82 @@
   </si>
   <si>
     <t>input:2</t>
+  </si>
+  <si>
+    <t>contextB:3</t>
+  </si>
+  <si>
+    <t>contextB</t>
+  </si>
+  <si>
+    <t>My age is {@sys.age:22}</t>
+  </si>
+  <si>
+    <t>My color is {@sys.color:blue}</t>
+  </si>
+  <si>
+    <t>contextC:3</t>
+  </si>
+  <si>
+    <t>contextC</t>
+  </si>
+  <si>
+    <t>Got it A</t>
+  </si>
+  <si>
+    <t>Got it B</t>
+  </si>
+  <si>
+    <t>Got it C</t>
+  </si>
+  <si>
+    <t>test.intentA</t>
+  </si>
+  <si>
+    <t>test.intentB</t>
+  </si>
+  <si>
+    <t>test.intentC</t>
+  </si>
+  <si>
+    <t>My name is {@sys.any:Steven}</t>
+  </si>
+  <si>
+    <t>sys.any:1</t>
+  </si>
+  <si>
+    <t>sys.color:1</t>
+  </si>
+  <si>
+    <t>{@sys.color:I'm sorry what is your color?}</t>
+  </si>
+  <si>
+    <t>{@sys.any:#contextB.sys_any:0:0}, {@sys.color:$sys_color:1:0}</t>
+  </si>
+  <si>
+    <t>test.parameter</t>
+  </si>
+  <si>
+    <t>contextD</t>
+  </si>
+  <si>
+    <t>event</t>
+  </si>
+  <si>
+    <t>I got your color</t>
+  </si>
+  <si>
+    <t>{@sys.age:{I'm sorry what is your age?}{could you repeat your age?}},{@sys.color:{I'm sorry what is your color?}}</t>
+  </si>
+  <si>
+    <t>{@sys.age:$sys_age:1:0},{@sys.any:#contextB.sys_any:1:0}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -866,6 +935,21 @@
       <sz val="11"/>
       <color rgb="FF2B313F"/>
       <name val="Roboto"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="34">
@@ -1231,7 +1315,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1242,10 +1326,17 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="42" applyAlignment="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3841,22 +3932,24 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08CBFBF2-BC64-48B4-A624-4A1B2A006627}">
-  <dimension ref="A1:K7"/>
+  <dimension ref="A1:L11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="6" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" style="6" customWidth="1"/>
-    <col min="5" max="16384" width="16.140625" style="1"/>
+    <col min="1" max="1" width="13.42578125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="13" style="10" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" style="10" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" style="10" customWidth="1"/>
+    <col min="5" max="7" width="12.7109375" style="6" customWidth="1"/>
+    <col min="8" max="11" width="25.7109375" style="6" customWidth="1"/>
+    <col min="12" max="16384" width="16.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>209</v>
       </c>
@@ -3888,59 +3981,182 @@
         <v>7</v>
       </c>
       <c r="K1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>226</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="C2" s="6">
-        <v>1</v>
-      </c>
-      <c r="D2" s="6">
-        <v>1</v>
-      </c>
-      <c r="E2" s="1" t="s">
+      <c r="C2" s="10">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10">
+        <v>1</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>227</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>228</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="6" t="s">
         <v>224</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="10">
         <v>0</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="10">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="6" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J7" s="1" t="s">
+    <row r="4" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
+        <v>238</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>241</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>239</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>233</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>236</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>240</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0</v>
+      </c>
+      <c r="E7" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="I7" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>244</v>
+      </c>
+      <c r="L7" s="6" t="s">
         <v>221</v>
       </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="J11" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>